<commit_message>
My final code for ParaBank Project
</commit_message>
<xml_diff>
--- a/src/main/java/com/parabank/qa/testdata/RegisrationDataExcelSheet.xlsx
+++ b/src/main/java/com/parabank/qa/testdata/RegisrationDataExcelSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdf9b91187737837/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaurr\AppData\Roaming\Microsoft\Windows\Network Shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70866D8D-A2CF-4C7E-9D4C-C4FCA38CBD98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA89180E-170F-4B11-80C4-976ED8259C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59429A26-6503-4973-9D94-3AF629D673F6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59429A26-6503-4973-9D94-3AF629D673F6}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistrationDataExcelSheet" sheetId="1" r:id="rId1"/>
@@ -176,7 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,7 +190,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -509,26 +508,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95EA223-B7BF-4F6E-AF21-CB58C72DDFBC}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -591,14 +590,14 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>12345</v>
       </c>
@@ -626,14 +625,14 @@
       <c r="I3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -661,14 +660,14 @@
       <c r="I4" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -696,14 +695,14 @@
       <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -728,14 +727,14 @@
       <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -763,14 +762,14 @@
       <c r="I7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -798,14 +797,14 @@
       <c r="I8" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -833,14 +832,14 @@
       <c r="I9" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -865,14 +864,14 @@
       <c r="I10" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -900,14 +899,14 @@
       <c r="I11" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -935,14 +934,14 @@
       <c r="I12" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -967,14 +966,14 @@
       <c r="I13" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1002,14 +1001,14 @@
       <c r="I14" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1037,14 +1036,14 @@
       <c r="I15" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1072,14 +1071,14 @@
       <c r="I16" t="s">
         <v>16</v>
       </c>
-      <c r="J16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1104,14 +1103,14 @@
       <c r="I17" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1139,14 +1138,14 @@
       <c r="I18" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1174,14 +1173,14 @@
       <c r="I19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1209,14 +1208,14 @@
       <c r="I20" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1241,14 +1240,14 @@
       <c r="I21" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1276,14 +1275,14 @@
       <c r="I22" t="s">
         <v>16</v>
       </c>
-      <c r="J22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1311,14 +1310,14 @@
       <c r="I23" t="s">
         <v>16</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1346,14 +1345,14 @@
       <c r="I24" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1381,14 +1380,14 @@
       <c r="I25" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -1416,14 +1415,14 @@
       <c r="I26" t="s">
         <v>16</v>
       </c>
-      <c r="J26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J26" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1448,14 +1447,14 @@
       <c r="I27" t="s">
         <v>16</v>
       </c>
-      <c r="J27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1483,14 +1482,14 @@
       <c r="I28" t="s">
         <v>16</v>
       </c>
-      <c r="J28" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1518,14 +1517,14 @@
       <c r="I29" t="s">
         <v>16</v>
       </c>
-      <c r="J29" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1553,14 +1552,14 @@
       <c r="I30" t="s">
         <v>16</v>
       </c>
-      <c r="J30" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -1585,14 +1584,14 @@
       <c r="I31" t="s">
         <v>16</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -1620,14 +1619,14 @@
       <c r="I32" t="s">
         <v>16</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1655,14 +1654,14 @@
       <c r="I33" t="s">
         <v>16</v>
       </c>
-      <c r="J33" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1690,14 +1689,14 @@
       <c r="I34" t="s">
         <v>16</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1725,14 +1724,14 @@
       <c r="I35" t="s">
         <v>16</v>
       </c>
-      <c r="J35" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -1760,14 +1759,14 @@
       <c r="I36" t="s">
         <v>16</v>
       </c>
-      <c r="J36" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -1795,14 +1794,14 @@
       <c r="I37" t="s">
         <v>16</v>
       </c>
-      <c r="J37" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J37" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1827,14 +1826,14 @@
       <c r="I38" t="s">
         <v>16</v>
       </c>
-      <c r="J38" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -1862,14 +1861,14 @@
       <c r="I39" t="s">
         <v>16</v>
       </c>
-      <c r="J39" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -1897,14 +1896,14 @@
       <c r="I40" t="s">
         <v>16</v>
       </c>
-      <c r="J40" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -1929,14 +1928,14 @@
       <c r="H41" s="2">
         <v>987456321</v>
       </c>
-      <c r="J41" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1964,12 +1963,12 @@
       <c r="I42" t="s">
         <v>16</v>
       </c>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="5"/>
+      <c r="K42" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>20</v>
       </c>
@@ -1997,10 +1996,10 @@
       <c r="I43" t="s">
         <v>16</v>
       </c>
-      <c r="J43" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K43" s="6"/>
+      <c r="J43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K43" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>